<commit_message>
Grouped java concepts into related packages
</commit_message>
<xml_diff>
--- a/amit-webservices/TestData.xlsx
+++ b/amit-webservices/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\amit-webservices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0B3A49-49C9-47E1-96CD-517FBC333066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A6CCFD-C481-4351-9EFA-1AF7DF0E1604}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreatePostRequest" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>userID</t>
   </si>
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,94 +415,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -512,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD2540C-8704-4B45-9472-62D530AD26DD}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Telstra interview prep, moved @DataProvider to common class
</commit_message>
<xml_diff>
--- a/amit-webservices/TestData.xlsx
+++ b/amit-webservices/TestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\amit-webservices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A6CCFD-C481-4351-9EFA-1AF7DF0E1604}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25056FDB-D3DE-484A-97FC-4C359D899811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreatePostRequest" sheetId="1" r:id="rId1"/>
     <sheet name="UpdatePostRequest" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateProduct" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>userID</t>
   </si>
@@ -53,16 +54,72 @@
   </si>
   <si>
     <t>body2</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>shipping</t>
+  </si>
+  <si>
+    <t>upc</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>Walkman</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Test pro</t>
+  </si>
+  <si>
+    <t>Sony</t>
+  </si>
+  <si>
+    <t>http://www.bestbuy.com/site/energizer-max-batteries-aa-4-pack/150115.p</t>
+  </si>
+  <si>
+    <t>http://img.bbystatic.com/BestBuy_US/images/products/4390/43900_sa.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -85,13 +142,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -372,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,4 +539,94 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30034E68-8676-452C-8029-DB43A1DB0DAA}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="64.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="63.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>4.99</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>41333821234</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>2021</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{0FB83E57-F7F7-4F18-B341-EBC4EB53D9BB}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{79BC8497-D0D9-4A0D-84E5-0BE90FB13E12}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>